<commit_message>
Use average mortality for cervical cancer grades. Adjusted scale-up for HPV vaccine uptake.
</commit_message>
<xml_diff>
--- a/HPVData.xlsx
+++ b/HPVData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\Model\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HPV" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="310">
   <si>
     <t>Age</t>
   </si>
@@ -956,6 +956,9 @@
   </si>
   <si>
     <t>Screening Coverage (within last 3 years)</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -9040,7 +9043,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S10" workbookViewId="0">
+    <sheetView topLeftCell="S10" workbookViewId="0">
       <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
@@ -9629,8 +9632,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9709,17 +9712,17 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="11">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="11">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="11">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="11">
         <v>2.93E-2</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -9757,17 +9760,17 @@
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="11">
         <f>3-2</f>
         <v>1</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="11">
         <v>1.4E-3</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="11">
         <v>7.7999999999999996E-3</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="11">
         <v>1.95E-2</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -9799,17 +9802,17 @@
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="11">
         <f>20-4</f>
         <v>16</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="11">
         <v>7.6E-3</v>
       </c>
       <c r="N5" s="4" t="s">
@@ -9832,17 +9835,17 @@
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="11">
         <f t="shared" ref="B6:B11" si="0">20-4</f>
         <v>16</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="11">
         <v>7.6E-3</v>
       </c>
       <c r="N6" s="4" t="s">
@@ -9862,17 +9865,17 @@
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="11">
         <v>7.6E-3</v>
       </c>
       <c r="T7" t="s">
@@ -9883,17 +9886,17 @@
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="11">
         <v>7.6E-3</v>
       </c>
       <c r="N8" s="3" t="s">
@@ -9910,17 +9913,17 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="11">
         <v>7.6E-3</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -9938,17 +9941,17 @@
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="11">
         <v>7.6E-3</v>
       </c>
       <c r="T10" s="20" t="s">
@@ -9963,17 +9966,17 @@
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="11">
         <v>7.6E-3</v>
       </c>
     </row>
@@ -9981,7 +9984,21 @@
       <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C13" s="55">
+        <f>AVERAGE(C3:C5)</f>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="D13" s="55">
+        <f>AVERAGE(D3:D5)</f>
+        <v>6.9666666666666661E-3</v>
+      </c>
+      <c r="E13" s="55">
+        <f>AVERAGE(E3:E5)</f>
+        <v>1.8800000000000001E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>

</xml_diff>

<commit_message>
Individuals on ART have same multipliers as CD4>500 individuals for HPV incidence/progression rates
</commit_message>
<xml_diff>
--- a/HPVData.xlsx
+++ b/HPVData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HPV" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="341">
   <si>
     <t>Age</t>
   </si>
@@ -1037,6 +1037,21 @@
   </si>
   <si>
     <t>HPV to Well (Natural Immunity)</t>
+  </si>
+  <si>
+    <t>Stage 1</t>
+  </si>
+  <si>
+    <t>Stage 2-3</t>
+  </si>
+  <si>
+    <t>Stage 4</t>
+  </si>
+  <si>
+    <t>Sankar</t>
+  </si>
+  <si>
+    <t>Sankar multiplied by Coghill 2015 HR (HIV+ vs HIV-)</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1707,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="88">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -3539,8 +3590,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4680,8 +4731,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BL86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9927,7 +9978,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:39" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="92" t="s">
         <v>262</v>
       </c>
@@ -10005,8 +10056,8 @@
         <v>0.63507222222222226</v>
       </c>
       <c r="G47" s="42">
-        <f t="array" ref="G47:G62">(F28:F43*2+G28:G43)/2</f>
-        <v>0.25831088888888887</v>
+        <f t="array" ref="G47:G62">(F28:F43+G28:G43)/2</f>
+        <v>0.15792799999999999</v>
       </c>
       <c r="H47" s="42">
         <f t="array" ref="H47:H62">(L28:L43+2*J28:J43)/2</f>
@@ -10034,11 +10085,11 @@
         <v>1.2063703703703702E-3</v>
       </c>
       <c r="AA47" s="42">
-        <v>0.63507222222222226</v>
+        <v>0.78637999999999997</v>
       </c>
       <c r="AB47" s="42">
-        <f t="array" ref="AB47:AB62">(AA28:AA43*2+AB28:AB43)/2</f>
-        <v>0.30386999999999997</v>
+        <f t="array" ref="AB47:AB62">(AA28:AA43+AB28:AB43)/2</f>
+        <v>0.1615095</v>
       </c>
       <c r="AC47" s="42">
         <f t="array" ref="AC47:AC62">(AG28:AG43+2*AE28:AE43)/2</f>
@@ -10069,7 +10120,7 @@
         <v>0.63507222222222226</v>
       </c>
       <c r="G48" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792799999999999</v>
       </c>
       <c r="H48" s="42">
         <v>0.32903294444444448</v>
@@ -10093,10 +10144,10 @@
         <v>1.2063703703703702E-3</v>
       </c>
       <c r="AA48" s="42">
-        <v>0.63507222222222226</v>
+        <v>0.78637999999999997</v>
       </c>
       <c r="AB48" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC48" s="42">
         <v>0.46084099999999995</v>
@@ -10125,7 +10176,7 @@
         <v>0.63507222222222226</v>
       </c>
       <c r="G49" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792799999999999</v>
       </c>
       <c r="H49" s="42">
         <v>0.32903294444444448</v>
@@ -10149,10 +10200,10 @@
         <v>1.2063703703703702E-3</v>
       </c>
       <c r="AA49" s="42">
-        <v>0.63507222222222226</v>
+        <v>0.78637999999999997</v>
       </c>
       <c r="AB49" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC49" s="42">
         <v>0.46084099999999995</v>
@@ -10181,7 +10232,7 @@
         <v>0.63507222222222226</v>
       </c>
       <c r="G50" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792799999999999</v>
       </c>
       <c r="H50" s="42">
         <v>0.32903294444444448</v>
@@ -10205,10 +10256,10 @@
         <v>1.2063703703703702E-3</v>
       </c>
       <c r="AA50" s="42">
-        <v>0.63507222222222226</v>
+        <v>0.78637999999999997</v>
       </c>
       <c r="AB50" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC50" s="42">
         <v>0.46084099999999995</v>
@@ -10237,7 +10288,7 @@
         <v>0.63507222222222226</v>
       </c>
       <c r="G51" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792799999999999</v>
       </c>
       <c r="H51" s="42">
         <v>0.32903294444444448</v>
@@ -10261,10 +10312,10 @@
         <v>1.2063703703703702E-3</v>
       </c>
       <c r="AA51" s="42">
-        <v>0.63507222222222226</v>
+        <v>0.78637999999999997</v>
       </c>
       <c r="AB51" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC51" s="42">
         <v>0.46084099999999995</v>
@@ -10293,7 +10344,7 @@
         <v>0.47923902777777783</v>
       </c>
       <c r="G52" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H52" s="42">
         <v>0.32903294444444448</v>
@@ -10317,10 +10368,10 @@
         <v>1.2754222222222222E-2</v>
       </c>
       <c r="AA52" s="42">
-        <v>0.47923902777777783</v>
+        <v>0.62775775</v>
       </c>
       <c r="AB52" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC52" s="42">
         <v>0.460841</v>
@@ -10349,7 +10400,7 @@
         <v>0.47923902777777783</v>
       </c>
       <c r="G53" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H53" s="42">
         <v>0.32903294444444448</v>
@@ -10373,10 +10424,10 @@
         <v>1.2754222222222222E-2</v>
       </c>
       <c r="AA53" s="42">
-        <v>0.47923902777777783</v>
+        <v>0.62775775</v>
       </c>
       <c r="AB53" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC53" s="42">
         <v>0.460841</v>
@@ -10405,7 +10456,7 @@
         <v>0.47923902777777783</v>
       </c>
       <c r="G54" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H54" s="42">
         <v>0.32903294444444448</v>
@@ -10429,10 +10480,10 @@
         <v>1.2754222222222222E-2</v>
       </c>
       <c r="AA54" s="42">
-        <v>0.47923902777777783</v>
+        <v>0.62775775</v>
       </c>
       <c r="AB54" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC54" s="42">
         <v>0.460841</v>
@@ -10461,7 +10512,7 @@
         <v>0.47923902777777783</v>
       </c>
       <c r="G55" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H55" s="42">
         <v>0.32903294444444448</v>
@@ -10485,10 +10536,10 @@
         <v>1.2754222222222222E-2</v>
       </c>
       <c r="AA55" s="42">
-        <v>0.47923902777777783</v>
+        <v>0.62775775</v>
       </c>
       <c r="AB55" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC55" s="42">
         <v>0.460841</v>
@@ -10517,7 +10568,7 @@
         <v>0.47923902777777783</v>
       </c>
       <c r="G56" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H56" s="42">
         <v>0.32903294444444448</v>
@@ -10541,10 +10592,10 @@
         <v>1.2754222222222222E-2</v>
       </c>
       <c r="AA56" s="42">
-        <v>0.47923902777777783</v>
+        <v>0.62775775</v>
       </c>
       <c r="AB56" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC56" s="42">
         <v>0.460841</v>
@@ -10573,7 +10624,7 @@
         <v>0.29655408333333333</v>
       </c>
       <c r="G57" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H57" s="42">
         <v>0.32903294444444448</v>
@@ -10597,10 +10648,10 @@
         <v>2.9281861111111109E-2</v>
       </c>
       <c r="AA57" s="42">
-        <v>0.29655408333333333</v>
+        <v>0.40971574999999999</v>
       </c>
       <c r="AB57" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC57" s="42">
         <v>0.460841</v>
@@ -10629,7 +10680,7 @@
         <v>0.29655408333333333</v>
       </c>
       <c r="G58" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H58" s="42">
         <v>0.32903294444444448</v>
@@ -10653,10 +10704,10 @@
         <v>2.9281861111111109E-2</v>
       </c>
       <c r="AA58" s="42">
-        <v>0.29655408333333333</v>
+        <v>0.40971574999999999</v>
       </c>
       <c r="AB58" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC58" s="42">
         <v>0.460841</v>
@@ -10685,7 +10736,7 @@
         <v>0.29655408333333333</v>
       </c>
       <c r="G59" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H59" s="42">
         <v>0.32903294444444448</v>
@@ -10709,10 +10760,10 @@
         <v>2.9281861111111109E-2</v>
       </c>
       <c r="AA59" s="42">
-        <v>0.29655408333333333</v>
+        <v>0.40971574999999999</v>
       </c>
       <c r="AB59" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC59" s="42">
         <v>0.460841</v>
@@ -10741,7 +10792,7 @@
         <v>0.29655408333333333</v>
       </c>
       <c r="G60" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792800000000001</v>
       </c>
       <c r="H60" s="42">
         <v>0.32903294444444448</v>
@@ -10765,10 +10816,10 @@
         <v>2.9281861111111109E-2</v>
       </c>
       <c r="AA60" s="42">
-        <v>0.29655408333333333</v>
+        <v>0.40971574999999999</v>
       </c>
       <c r="AB60" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC60" s="42">
         <v>0.460841</v>
@@ -10797,7 +10848,7 @@
         <v>0.26289588888888893</v>
       </c>
       <c r="G61" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792799999999999</v>
       </c>
       <c r="H61" s="42">
         <v>0.32903294444444448</v>
@@ -10821,10 +10872,10 @@
         <v>3.4510925925925924E-2</v>
       </c>
       <c r="AA61" s="42">
-        <v>0.26289588888888893</v>
+        <v>0.36699399999999999</v>
       </c>
       <c r="AB61" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC61" s="42">
         <v>0.46084099999999995</v>
@@ -10853,7 +10904,7 @@
         <v>0.26289588888888893</v>
       </c>
       <c r="G62" s="42">
-        <v>0.25831088888888887</v>
+        <v>0.15792799999999999</v>
       </c>
       <c r="H62" s="42">
         <v>0.32903294444444448</v>
@@ -10877,10 +10928,10 @@
         <v>3.4510925925925924E-2</v>
       </c>
       <c r="AA62" s="42">
-        <v>0.26289588888888893</v>
+        <v>0.36699399999999999</v>
       </c>
       <c r="AB62" s="42">
-        <v>0.30386999999999997</v>
+        <v>0.1615095</v>
       </c>
       <c r="AC62" s="42">
         <v>0.46084099999999995</v>
@@ -10913,6 +10964,7 @@
         <v>201</v>
       </c>
       <c r="D68" s="57">
+        <f>0.6</f>
         <v>0.6</v>
       </c>
     </row>
@@ -10923,6 +10975,7 @@
         <v>241</v>
       </c>
       <c r="D69" s="58">
+        <f>0.55</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -10933,6 +10986,7 @@
         <v>199</v>
       </c>
       <c r="D70" s="58">
+        <f>0.45</f>
         <v>0.45</v>
       </c>
     </row>
@@ -10943,6 +10997,7 @@
         <v>243</v>
       </c>
       <c r="D71" s="59">
+        <f>0.3</f>
         <v>0.3</v>
       </c>
     </row>
@@ -11068,427 +11123,427 @@
     <sortCondition descending="1" ref="H102"/>
   </sortState>
   <conditionalFormatting sqref="BI17:BI18">
-    <cfRule type="cellIs" dxfId="84" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="44" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:BL4">
-    <cfRule type="cellIs" dxfId="83" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="43" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:BL16">
-    <cfRule type="cellIs" dxfId="82" priority="85" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="85" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB2:BH2 BJ2:BL2">
-    <cfRule type="cellIs" dxfId="81" priority="84" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="84" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW2:BA2">
-    <cfRule type="cellIs" dxfId="80" priority="83" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="83" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AF2">
-    <cfRule type="cellIs" dxfId="79" priority="80" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="80" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR2:AV2">
-    <cfRule type="cellIs" dxfId="78" priority="82" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="82" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:AA2">
-    <cfRule type="cellIs" dxfId="77" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="79" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG2:AQ2">
-    <cfRule type="cellIs" dxfId="76" priority="81" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="81" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:V2">
-    <cfRule type="cellIs" dxfId="75" priority="78" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="78" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:K2">
-    <cfRule type="cellIs" dxfId="74" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="77" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F2">
-    <cfRule type="cellIs" dxfId="73" priority="76" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="76" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI2">
-    <cfRule type="cellIs" dxfId="72" priority="75" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="75" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:E18">
-    <cfRule type="cellIs" dxfId="71" priority="67" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="67" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:I18">
-    <cfRule type="cellIs" dxfId="70" priority="66" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="66" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ17:AJ18">
-    <cfRule type="cellIs" dxfId="69" priority="63" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="63" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:J18">
-    <cfRule type="cellIs" dxfId="68" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="65" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO17:AO18">
-    <cfRule type="cellIs" dxfId="67" priority="62" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="62" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ17:AQ18 AK17:AN18 AG17:AI18">
-    <cfRule type="cellIs" dxfId="66" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="64" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C18">
-    <cfRule type="cellIs" dxfId="65" priority="68" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="68" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP17:AP18">
-    <cfRule type="cellIs" dxfId="64" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="61" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF17:AF18 AB17:AC18">
-    <cfRule type="cellIs" dxfId="63" priority="60" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="60" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V17:V18 P17:S18 L17:N18">
-    <cfRule type="cellIs" dxfId="62" priority="74" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="74" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O18">
-    <cfRule type="cellIs" dxfId="61" priority="73" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="73" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T17:T18">
-    <cfRule type="cellIs" dxfId="60" priority="72" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="72" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U17:U18">
-    <cfRule type="cellIs" dxfId="59" priority="71" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="71" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD17:AD18">
-    <cfRule type="cellIs" dxfId="58" priority="56" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="56" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K18 G17:H18">
-    <cfRule type="cellIs" dxfId="57" priority="70" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="70" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK17:BK18">
-    <cfRule type="cellIs" dxfId="56" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="51" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL17:BL18 BF17:BH18 BB17:BD18">
-    <cfRule type="cellIs" dxfId="55" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="54" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D18 F17:F18 B17:B18">
-    <cfRule type="cellIs" dxfId="54" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="69" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY17:AY18">
-    <cfRule type="cellIs" dxfId="53" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="46" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ17:AZ18">
-    <cfRule type="cellIs" dxfId="52" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="45" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y17:Y18 AA17:AA18 W17:W18">
-    <cfRule type="cellIs" dxfId="51" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="59" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X17:X18">
-    <cfRule type="cellIs" dxfId="50" priority="58" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="58" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17:Z18">
-    <cfRule type="cellIs" dxfId="49" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="57" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE17:AE18">
-    <cfRule type="cellIs" dxfId="48" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="55" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE17:BE18">
-    <cfRule type="cellIs" dxfId="47" priority="53" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="53" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ17:BJ18">
-    <cfRule type="cellIs" dxfId="46" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="52" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA17:BA18 AW17:AX18">
-    <cfRule type="cellIs" dxfId="45" priority="50" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT17:AT18 AV17:AV18 AR17:AR18">
-    <cfRule type="cellIs" dxfId="44" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS17:AS18">
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU17:AU18">
-    <cfRule type="cellIs" dxfId="42" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W28:W29">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="40" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W30:W41">
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W42:W43">
-    <cfRule type="cellIs" dxfId="39" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="41" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X28:X29">
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X30:X41">
-    <cfRule type="cellIs" dxfId="37" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X42:X43">
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y28:Y29">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y30:Y41">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="36" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y42:Y43">
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA28:AA29">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA30:AA41">
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA42:AA43">
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB28:AB29">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB30:AB41">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB42:AB43">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC28:AC29">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC30:AC41">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC42:AC43">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD28:AD29">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30:AD41">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD42:AD43">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE28:AE29">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE30:AE41">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE42:AE43">
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF28:AF29">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF30:AF41">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF42:AF43">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG28:AG29">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG30:AG41">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG42:AG43">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH28:AH29">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH30:AH41">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH42:AH43">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK42:AK43">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28:AK29">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK30:AK41">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL28:AL29">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL30:AL41">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL42:AL43">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM28:AM29">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM30:AM41">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM42:AM43">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12091,8 +12146,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12446,15 +12501,15 @@
       <c r="A13" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="64">
         <f>AVERAGE(C3:C5)</f>
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="64">
         <f>AVERAGE(D3:D5)</f>
         <v>6.9666666666666661E-3</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="64">
         <f>AVERAGE(E3:E5)</f>
         <v>1.8800000000000001E-2</v>
       </c>
@@ -12468,6 +12523,51 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>336</v>
+      </c>
+      <c r="D23" t="s">
+        <v>337</v>
+      </c>
+      <c r="E23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>339</v>
+      </c>
+      <c r="C24" s="42">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="D24" s="42">
+        <v>1.2513E-2</v>
+      </c>
+      <c r="E24" s="42">
+        <v>4.3395000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" t="s">
+        <v>340</v>
+      </c>
+      <c r="C25" s="42">
+        <v>8.6829999999999997E-3</v>
+      </c>
+      <c r="D25" s="42">
+        <v>2.0896999999999999E-2</v>
+      </c>
+      <c r="E25" s="42">
+        <v>7.2469000000000006E-2</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Modified age groups used to calculate incidence
</commit_message>
<xml_diff>
--- a/HPVData.xlsx
+++ b/HPVData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HPV" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="346">
   <si>
     <t>Age</t>
   </si>
@@ -1039,9 +1039,6 @@
     <t>Sankar</t>
   </si>
   <si>
-    <t>Sankar multiplied by Coghill 2015 HR (HIV+ vs HIV-)</t>
-  </si>
-  <si>
     <t>Vaccine types</t>
   </si>
   <si>
@@ -1049,6 +1046,27 @@
   </si>
   <si>
     <t>HPV to Well (Natural Immunity)</t>
+  </si>
+  <si>
+    <t>HIV + on ART</t>
+  </si>
+  <si>
+    <t>HIV + CD4 &gt;500</t>
+  </si>
+  <si>
+    <t>HIV + CD4 350-500</t>
+  </si>
+  <si>
+    <t>HIV + CD4 250-350</t>
+  </si>
+  <si>
+    <t>HIV + CD4 &lt;250</t>
+  </si>
+  <si>
+    <t>Dryden-peterson</t>
+  </si>
+  <si>
+    <t>Montly CC Mortality Rates</t>
   </si>
 </sst>
 </file>
@@ -2751,23 +2769,23 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" customWidth="1"/>
-    <col min="7" max="7" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="16" max="16" width="15.54296875" customWidth="1"/>
-    <col min="17" max="18" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" customWidth="1"/>
-    <col min="21" max="21" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="18" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>146</v>
       </c>
@@ -2778,7 +2796,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>147</v>
       </c>
@@ -2828,7 +2846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>16</v>
       </c>
@@ -2878,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>18</v>
       </c>
@@ -2928,7 +2946,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>31</v>
       </c>
@@ -2976,7 +2994,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>33</v>
       </c>
@@ -3023,7 +3041,7 @@
         <v>14.04</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3056,7 +3074,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>39</v>
       </c>
@@ -3097,7 +3115,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>51</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>56</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G11" s="24" t="s">
         <v>180</v>
       </c>
@@ -3145,7 +3163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>147</v>
       </c>
@@ -3184,7 +3202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>160</v>
       </c>
@@ -3227,7 +3245,7 @@
         <v>0.24271844660194175</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>149</v>
       </c>
@@ -3270,7 +3288,7 @@
         <v>0.12376237623762376</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>234</v>
       </c>
@@ -3302,7 +3320,7 @@
         <v>7.1225071225071226E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G16" s="4" t="s">
         <v>159</v>
       </c>
@@ -3316,7 +3334,7 @@
         <v>1.7130000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G17" s="11" t="s">
         <v>162</v>
       </c>
@@ -3330,7 +3348,7 @@
         <v>1.863</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="11" t="s">
         <v>54</v>
       </c>
@@ -3347,7 +3365,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="44" t="s">
         <v>238</v>
@@ -3370,7 +3388,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
       <c r="B20" s="7" t="s">
         <v>47</v>
@@ -3400,7 +3418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
         <v>198</v>
       </c>
@@ -3430,7 +3448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>199</v>
       </c>
@@ -3462,7 +3480,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
         <v>241</v>
       </c>
@@ -3499,7 +3517,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="48" t="s">
         <v>201</v>
       </c>
@@ -3528,7 +3546,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G25" s="9" t="s">
         <v>183</v>
       </c>
@@ -3539,7 +3557,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G27" s="24" t="s">
         <v>184</v>
       </c>
@@ -3547,7 +3565,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>185</v>
       </c>
@@ -3561,7 +3579,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G29" s="4" t="s">
         <v>169</v>
       </c>
@@ -3585,7 +3603,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G30" s="4" t="s">
         <v>170</v>
       </c>
@@ -3609,7 +3627,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G31" s="11" t="s">
         <v>187</v>
       </c>
@@ -3634,7 +3652,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q32" t="s">
         <v>201</v>
       </c>
@@ -3642,7 +3660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G34" s="24" t="s">
         <v>179</v>
       </c>
@@ -3650,7 +3668,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G35" s="13" t="s">
         <v>147</v>
       </c>
@@ -3676,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G36" s="4" t="s">
         <v>47</v>
       </c>
@@ -3709,7 +3727,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G37" s="4" t="s">
         <v>157</v>
       </c>
@@ -3742,7 +3760,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G38" s="4" t="s">
         <v>158</v>
       </c>
@@ -3763,7 +3781,7 @@
         <v>1.925E-2</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G39" s="4" t="s">
         <v>159</v>
       </c>
@@ -3777,7 +3795,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G40" s="11" t="s">
         <v>162</v>
       </c>
@@ -3791,7 +3809,7 @@
         <v>0.128</v>
       </c>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G41" s="11" t="s">
         <v>54</v>
       </c>
@@ -3805,7 +3823,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G42" s="11" t="s">
         <v>163</v>
       </c>
@@ -3819,12 +3837,12 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G45" s="24" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G46" s="4" t="s">
         <v>62</v>
       </c>
@@ -3835,7 +3853,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G47" s="4">
         <v>0.48</v>
       </c>
@@ -3861,17 +3879,17 @@
       <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="55"/>
+    <col min="1" max="16384" width="8.7109375" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:64" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="58" t="s">
         <v>262</v>
       </c>
@@ -4065,7 +4083,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="55" t="s">
         <v>309</v>
       </c>
@@ -4259,7 +4277,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
         <v>310</v>
       </c>
@@ -4453,7 +4471,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72" t="s">
         <v>305</v>
       </c>
@@ -4647,7 +4665,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
         <v>229</v>
       </c>
@@ -4841,7 +4859,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
         <v>230</v>
       </c>
@@ -5035,7 +5053,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>306</v>
       </c>
@@ -5229,7 +5247,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
         <v>10</v>
       </c>
@@ -5423,7 +5441,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>11</v>
       </c>
@@ -5617,7 +5635,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>12</v>
       </c>
@@ -5811,7 +5829,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>13</v>
       </c>
@@ -6005,7 +6023,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>232</v>
       </c>
@@ -6199,7 +6217,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
         <v>233</v>
       </c>
@@ -6393,7 +6411,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
         <v>253</v>
       </c>
@@ -6587,7 +6605,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
         <v>254</v>
       </c>
@@ -6781,7 +6799,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="78" t="s">
         <v>307</v>
       </c>
@@ -6975,7 +6993,7 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="55" t="s">
         <v>308</v>
       </c>
@@ -7169,12 +7187,12 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>47</v>
       </c>
@@ -7183,7 +7201,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="55" t="s">
         <v>157</v>
       </c>
@@ -7192,7 +7210,7 @@
         <v>0.22222222222222224</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="55" t="s">
         <v>322</v>
       </c>
@@ -7201,7 +7219,7 @@
         <v>0.22222222222222224</v>
       </c>
     </row>
-    <row r="27" spans="1:64" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:64" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="84" t="s">
         <v>262</v>
       </c>
@@ -7311,7 +7329,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="28" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="55" t="s">
         <v>309</v>
       </c>
@@ -7441,7 +7459,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="71" t="s">
         <v>310</v>
       </c>
@@ -7551,7 +7569,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="72" t="s">
         <v>305</v>
       </c>
@@ -7661,7 +7679,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="55" t="s">
         <v>229</v>
       </c>
@@ -7771,7 +7789,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>230</v>
       </c>
@@ -7881,7 +7899,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
         <v>306</v>
       </c>
@@ -7991,7 +8009,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="55" t="s">
         <v>10</v>
       </c>
@@ -8101,7 +8119,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>11</v>
       </c>
@@ -8211,7 +8229,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
         <v>12</v>
       </c>
@@ -8321,7 +8339,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="55" t="s">
         <v>13</v>
       </c>
@@ -8431,7 +8449,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
         <v>232</v>
       </c>
@@ -8541,7 +8559,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="55" t="s">
         <v>233</v>
       </c>
@@ -8651,7 +8669,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="55" t="s">
         <v>253</v>
       </c>
@@ -8761,7 +8779,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="55" t="s">
         <v>254</v>
       </c>
@@ -8871,7 +8889,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="78" t="s">
         <v>307</v>
       </c>
@@ -8981,7 +8999,7 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="55" t="s">
         <v>308</v>
       </c>
@@ -9091,15 +9109,15 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="55" t="s">
+        <v>336</v>
+      </c>
+      <c r="V45" s="55" t="s">
         <v>337</v>
       </c>
-      <c r="V45" s="55" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="46" spans="1:39" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:39" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="84" t="s">
         <v>262</v>
       </c>
@@ -9116,7 +9134,7 @@
         <v>329</v>
       </c>
       <c r="F46" s="85" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G46" s="85" t="s">
         <v>318</v>
@@ -9143,7 +9161,7 @@
         <v>329</v>
       </c>
       <c r="AA46" s="85" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB46" s="85" t="s">
         <v>318</v>
@@ -9155,7 +9173,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" s="55" t="s">
         <v>309</v>
       </c>
@@ -9221,7 +9239,7 @@
         <v>0.12066450000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" s="71" t="s">
         <v>310</v>
       </c>
@@ -9277,7 +9295,7 @@
         <v>0.12066450000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="72" t="s">
         <v>305</v>
       </c>
@@ -9333,7 +9351,7 @@
         <v>0.12066450000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="55" t="s">
         <v>229</v>
       </c>
@@ -9389,7 +9407,7 @@
         <v>0.12066450000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>230</v>
       </c>
@@ -9445,7 +9463,7 @@
         <v>0.12066450000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>306</v>
       </c>
@@ -9501,7 +9519,7 @@
         <v>9.0632875000000002E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="55" t="s">
         <v>10</v>
       </c>
@@ -9557,7 +9575,7 @@
         <v>9.0632875000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" s="55" t="s">
         <v>11</v>
       </c>
@@ -9613,7 +9631,7 @@
         <v>9.0632875000000002E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>12</v>
       </c>
@@ -9669,7 +9687,7 @@
         <v>9.0632875000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="55" t="s">
         <v>13</v>
       </c>
@@ -9725,7 +9743,7 @@
         <v>9.0632875000000002E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="55" t="s">
         <v>232</v>
       </c>
@@ -9781,7 +9799,7 @@
         <v>3.3547999999999994E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" s="55" t="s">
         <v>233</v>
       </c>
@@ -9837,7 +9855,7 @@
         <v>3.3547999999999994E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" s="55" t="s">
         <v>253</v>
       </c>
@@ -9893,7 +9911,7 @@
         <v>3.3547999999999994E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="55" t="s">
         <v>254</v>
       </c>
@@ -9949,7 +9967,7 @@
         <v>3.3547999999999994E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" s="78" t="s">
         <v>307</v>
       </c>
@@ -10005,7 +10023,7 @@
         <v>1.7070999999999999E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" s="55" t="s">
         <v>308</v>
       </c>
@@ -10061,8 +10079,8 @@
         <v>1.7070999999999999E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="86"/>
       <c r="B67" s="87"/>
       <c r="C67" s="88" t="s">
@@ -10070,7 +10088,7 @@
       </c>
       <c r="D67" s="89"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="90"/>
       <c r="C68" s="91" t="s">
         <v>201</v>
@@ -10080,7 +10098,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="90"/>
       <c r="C69" s="91" t="s">
         <v>241</v>
@@ -10090,7 +10108,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="90"/>
       <c r="C70" s="91" t="s">
         <v>199</v>
@@ -10100,7 +10118,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="94"/>
       <c r="B71" s="95"/>
       <c r="C71" s="96" t="s">
@@ -10111,12 +10129,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="55" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="98" t="s">
         <v>201</v>
       </c>
@@ -10127,7 +10145,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="90" t="s">
         <v>241</v>
       </c>
@@ -10138,7 +10156,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="90" t="s">
         <v>199</v>
       </c>
@@ -10146,7 +10164,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="94" t="s">
         <v>198</v>
       </c>
@@ -10154,12 +10172,12 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="55" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="98" t="s">
         <v>201</v>
       </c>
@@ -10170,7 +10188,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="90" t="s">
         <v>241</v>
       </c>
@@ -10181,7 +10199,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="90" t="s">
         <v>199</v>
       </c>
@@ -10192,7 +10210,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="94" t="s">
         <v>198</v>
       </c>
@@ -10203,7 +10221,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D85" s="57" t="s">
         <v>250</v>
       </c>
@@ -10226,27 +10244,27 @@
       <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.1796875" customWidth="1"/>
-    <col min="20" max="23" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" customWidth="1"/>
+    <col min="20" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" customWidth="1"/>
     <col min="26" max="26" width="32" customWidth="1"/>
-    <col min="27" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.453125" customWidth="1"/>
+    <col min="27" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>58</v>
       </c>
@@ -10273,7 +10291,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>57</v>
       </c>
@@ -10328,7 +10346,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>60</v>
       </c>
@@ -10390,7 +10408,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
@@ -10446,7 +10464,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>106</v>
       </c>
@@ -10481,7 +10499,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="M6" s="4" t="s">
         <v>114</v>
@@ -10520,7 +10538,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="M7" s="3" t="s">
         <v>118</v>
       </c>
@@ -10551,7 +10569,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S8" s="3" t="s">
         <v>129</v>
       </c>
@@ -10576,7 +10594,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="Y9" s="3" t="s">
         <v>138</v>
       </c>
@@ -10584,12 +10602,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AD10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S11" s="24" t="s">
         <v>130</v>
       </c>
@@ -10600,7 +10618,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K12" s="15"/>
       <c r="T12" s="24" t="s">
         <v>124</v>
@@ -10617,7 +10635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S13" s="21" t="s">
         <v>119</v>
       </c>
@@ -10640,7 +10658,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S14" s="13" t="s">
         <v>120</v>
       </c>
@@ -10657,7 +10675,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S15" s="13" t="s">
         <v>121</v>
       </c>
@@ -10670,7 +10688,7 @@
       </c>
       <c r="W15" s="4"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S16" s="13" t="s">
         <v>122</v>
       </c>
@@ -10689,7 +10707,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="17" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S17" s="13" t="s">
         <v>123</v>
       </c>
@@ -10709,18 +10727,18 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S18" s="3" t="s">
         <v>129</v>
       </c>
       <c r="AA18" s="15"/>
     </row>
-    <row r="20" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S20" s="24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="19:27" x14ac:dyDescent="0.25">
       <c r="T21" s="24" t="s">
         <v>124</v>
       </c>
@@ -10730,7 +10748,7 @@
       </c>
       <c r="W21" s="24"/>
     </row>
-    <row r="22" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S22" s="21" t="s">
         <v>119</v>
       </c>
@@ -10747,7 +10765,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S23" s="13" t="s">
         <v>120</v>
       </c>
@@ -10764,7 +10782,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="24" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S24" s="13" t="s">
         <v>121</v>
       </c>
@@ -10777,7 +10795,7 @@
       </c>
       <c r="W24" s="4"/>
     </row>
-    <row r="25" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S25" s="13" t="s">
         <v>123</v>
       </c>
@@ -10794,7 +10812,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="26" spans="19:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="19:27" x14ac:dyDescent="0.25">
       <c r="S26" s="3" t="s">
         <v>129</v>
       </c>
@@ -10809,21 +10827,22 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="6" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -10840,7 +10859,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -10887,7 +10906,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -10935,7 +10954,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -10977,7 +10996,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -11010,7 +11029,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -11040,7 +11059,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -11061,7 +11080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -11088,7 +11107,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -11116,7 +11135,7 @@
         <v>0.13824884792626729</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
@@ -11141,7 +11160,7 @@
         <v>9.8360655737704916E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -11159,10 +11178,10 @@
         <v>7.6E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>261</v>
       </c>
@@ -11179,67 +11198,126 @@
         <v>1.8800000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>332</v>
       </c>
-      <c r="D23" s="55" t="s">
+      <c r="C23" t="s">
         <v>333</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="D23" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="55" t="s">
-        <v>335</v>
-      </c>
-      <c r="C24" s="56">
-        <v>5.1999999999999998E-3</v>
-      </c>
-      <c r="D24" s="56">
-        <v>1.2513E-2</v>
-      </c>
-      <c r="E24" s="56">
-        <v>4.3395000000000003E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="55" t="s">
-        <v>336</v>
-      </c>
-      <c r="C25" s="56">
-        <v>8.6829999999999997E-3</v>
-      </c>
-      <c r="D25" s="56">
-        <v>2.0896999999999999E-2</v>
-      </c>
-      <c r="E25" s="56">
-        <v>7.2469000000000006E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>340</v>
+      </c>
+      <c r="B24" s="41">
+        <v>8.0070000000000002E-3</v>
+      </c>
+      <c r="C24" s="41">
+        <v>1.9269999999999999E-2</v>
+      </c>
+      <c r="D24" s="41">
+        <v>6.6827999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>341</v>
+      </c>
+      <c r="B25" s="41">
+        <v>9.7230000000000007E-3</v>
+      </c>
+      <c r="C25" s="41">
+        <v>2.3399E-2</v>
+      </c>
+      <c r="D25" s="41">
+        <v>8.1147999999999998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>342</v>
+      </c>
+      <c r="B26" s="41">
+        <v>1.1802999999999999E-2</v>
+      </c>
+      <c r="C26" s="41">
+        <v>2.8403999999999999E-2</v>
+      </c>
+      <c r="D26" s="41">
+        <v>9.8505999999999996E-2</v>
+      </c>
       <c r="N26" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B27" s="41">
+        <v>1.4298999999999999E-2</v>
+      </c>
+      <c r="C27" s="41">
+        <v>3.4410999999999997E-2</v>
+      </c>
+      <c r="D27" s="41">
+        <v>0.119336</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>339</v>
+      </c>
+      <c r="B28" s="41">
+        <v>8.0070000000000002E-3</v>
+      </c>
+      <c r="C28" s="41">
+        <v>1.9269999999999999E-2</v>
+      </c>
+      <c r="D28" s="41">
+        <v>6.6827999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="41">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="C29" s="41">
+        <v>1.2513E-2</v>
+      </c>
+      <c r="D29" s="41">
+        <v>4.3395000000000003E-2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -11257,28 +11335,28 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.54296875" customWidth="1"/>
-    <col min="25" max="25" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.54296875" customWidth="1"/>
-    <col min="31" max="31" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.5703125" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" customWidth="1"/>
+    <col min="31" max="31" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -11303,7 +11381,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -11366,7 +11444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -11430,7 +11508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
@@ -11494,7 +11572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -11534,7 +11612,7 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>38</v>
       </c>
@@ -11587,7 +11665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -11629,7 +11707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -11668,7 +11746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -11692,7 +11770,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -11725,7 +11803,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -11767,7 +11845,7 @@
         <v>0.74550000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -11796,7 +11874,7 @@
         <v>0.751</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -11827,7 +11905,7 @@
         <v>0.24271844660194175</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -11851,7 +11929,7 @@
         <v>0.12376237623762376</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H15" s="7"/>
       <c r="N15" s="4" t="s">
         <v>67</v>
@@ -11869,21 +11947,21 @@
         <v>7.1225071225071226E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H16" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
@@ -11891,7 +11969,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
@@ -11902,7 +11980,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
@@ -11913,12 +11991,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>47</v>
       </c>
@@ -11929,7 +12007,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>1</v>
       </c>
@@ -11946,7 +12024,7 @@
         <v>9.0833333333333339E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
@@ -11963,22 +12041,22 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>141</v>
       </c>
@@ -11986,7 +12064,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="22" t="s">
         <v>62</v>
       </c>
@@ -12006,7 +12084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>83</v>
       </c>
@@ -12035,7 +12113,7 @@
         <v>7.5000000000000002E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>88</v>
       </c>
@@ -12064,7 +12142,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>89</v>
       </c>
@@ -12093,7 +12171,7 @@
         <v>1.7499999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>91</v>
       </c>
@@ -12123,7 +12201,7 @@
         <v>3.2500000000000003E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>142</v>
       </c>
@@ -12131,7 +12209,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="22" t="s">
         <v>62</v>
       </c>
@@ -12151,7 +12229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>83</v>
       </c>
@@ -12180,7 +12258,7 @@
         <v>1.25E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>88</v>
       </c>
@@ -12209,7 +12287,7 @@
         <v>3.4999999999999996E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>89</v>
       </c>
@@ -12238,7 +12316,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>91</v>
       </c>
@@ -12267,21 +12345,21 @@
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>90</v>
       </c>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G51" s="23"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>92</v>
       </c>
@@ -12295,7 +12373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>96</v>
       </c>
@@ -12309,7 +12387,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>94</v>
       </c>
@@ -12323,7 +12401,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>95</v>
       </c>
@@ -12337,12 +12415,12 @@
         <v>13.42</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>92</v>
       </c>
@@ -12356,7 +12434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>96</v>
       </c>
@@ -12370,7 +12448,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>94</v>
       </c>
@@ -12384,7 +12462,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>95</v>
       </c>
@@ -12414,14 +12492,14 @@
       <selection activeCell="B3" sqref="B3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>237</v>
       </c>
@@ -12429,7 +12507,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>229</v>
       </c>
@@ -12443,7 +12521,7 @@
         <v>16.6279069767441</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -12457,7 +12535,7 @@
         <v>39.999999999999901</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>231</v>
       </c>
@@ -12471,7 +12549,7 @@
         <v>45.232558139534802</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -12485,7 +12563,7 @@
         <v>43.139534883720899</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -12499,7 +12577,7 @@
         <v>39.651162790697597</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -12513,7 +12591,7 @@
         <v>24.651162790697601</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
3 HPV categories now: 16/18, non-4v covered type, non-vaccine type.
</commit_message>
<xml_diff>
--- a/HPVData.xlsx
+++ b/HPVData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="350">
   <si>
     <t>Age</t>
   </si>
@@ -1039,9 +1039,6 @@
     <t>Sankar</t>
   </si>
   <si>
-    <t>Vaccine types</t>
-  </si>
-  <si>
     <t>Non-Vaccine Types</t>
   </si>
   <si>
@@ -1076,6 +1073,12 @@
   </si>
   <si>
     <t>4v-Type Subgroup weighting</t>
+  </si>
+  <si>
+    <t>Vaccine types (16/18)</t>
+  </si>
+  <si>
+    <t>Vaccine type (non-16/18)</t>
   </si>
 </sst>
 </file>
@@ -2791,19 +2794,19 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+    <col min="7" max="7" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="18" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.54296875" customWidth="1"/>
+    <col min="17" max="18" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.54296875" customWidth="1"/>
+    <col min="21" max="21" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>146</v>
       </c>
@@ -2814,7 +2817,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>147</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>16</v>
       </c>
@@ -2914,7 +2917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>18</v>
       </c>
@@ -2964,7 +2967,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>31</v>
       </c>
@@ -3012,7 +3015,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>33</v>
       </c>
@@ -3059,7 +3062,7 @@
         <v>14.04</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3092,7 +3095,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>39</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>51</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>56</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G11" s="24" t="s">
         <v>180</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>147</v>
       </c>
@@ -3220,7 +3223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>160</v>
       </c>
@@ -3263,7 +3266,7 @@
         <v>0.24271844660194175</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>149</v>
       </c>
@@ -3306,7 +3309,7 @@
         <v>0.12376237623762376</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>234</v>
       </c>
@@ -3338,7 +3341,7 @@
         <v>7.1225071225071226E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G16" s="4" t="s">
         <v>159</v>
       </c>
@@ -3352,7 +3355,7 @@
         <v>1.7130000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G17" s="11" t="s">
         <v>162</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>1.863</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G18" s="11" t="s">
         <v>54</v>
       </c>
@@ -3383,7 +3386,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="43"/>
       <c r="B19" s="44" t="s">
         <v>238</v>
@@ -3406,7 +3409,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="46"/>
       <c r="B20" s="7" t="s">
         <v>47</v>
@@ -3436,7 +3439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="46" t="s">
         <v>198</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="46" t="s">
         <v>199</v>
       </c>
@@ -3498,7 +3501,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="46" t="s">
         <v>241</v>
       </c>
@@ -3535,7 +3538,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="48" t="s">
         <v>201</v>
       </c>
@@ -3564,7 +3567,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G25" s="9" t="s">
         <v>183</v>
       </c>
@@ -3575,7 +3578,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G27" s="24" t="s">
         <v>184</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="H28" t="s">
         <v>185</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G29" s="4" t="s">
         <v>169</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G30" s="4" t="s">
         <v>170</v>
       </c>
@@ -3645,7 +3648,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G31" s="11" t="s">
         <v>187</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="Q32" t="s">
         <v>201</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G34" s="24" t="s">
         <v>179</v>
       </c>
@@ -3686,7 +3689,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G35" s="13" t="s">
         <v>147</v>
       </c>
@@ -3712,7 +3715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G36" s="4" t="s">
         <v>47</v>
       </c>
@@ -3745,7 +3748,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G37" s="4" t="s">
         <v>157</v>
       </c>
@@ -3778,7 +3781,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G38" s="4" t="s">
         <v>158</v>
       </c>
@@ -3799,7 +3802,7 @@
         <v>1.925E-2</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G39" s="4" t="s">
         <v>159</v>
       </c>
@@ -3813,7 +3816,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G40" s="11" t="s">
         <v>162</v>
       </c>
@@ -3827,7 +3830,7 @@
         <v>0.128</v>
       </c>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G41" s="11" t="s">
         <v>54</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G42" s="11" t="s">
         <v>163</v>
       </c>
@@ -3855,12 +3858,12 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G45" s="24" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G46" s="4" t="s">
         <v>62</v>
       </c>
@@ -3871,7 +3874,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G47" s="4">
         <v>0.48</v>
       </c>
@@ -3893,21 +3896,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BL85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="AG52" sqref="AG52"/>
+    <sheetView tabSelected="1" topLeftCell="O43" workbookViewId="0">
+      <selection activeCell="AF58" sqref="AF58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="55"/>
+    <col min="1" max="16384" width="8.7265625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="57" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="58" t="s">
         <v>262</v>
       </c>
@@ -4101,7 +4104,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="55" t="s">
         <v>309</v>
       </c>
@@ -4295,7 +4298,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="71" t="s">
         <v>310</v>
       </c>
@@ -4489,7 +4492,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="72" t="s">
         <v>305</v>
       </c>
@@ -4683,7 +4686,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="55" t="s">
         <v>229</v>
       </c>
@@ -4877,7 +4880,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A7" s="55" t="s">
         <v>230</v>
       </c>
@@ -5071,7 +5074,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A8" s="55" t="s">
         <v>306</v>
       </c>
@@ -5265,7 +5268,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A9" s="55" t="s">
         <v>10</v>
       </c>
@@ -5459,7 +5462,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A10" s="55" t="s">
         <v>11</v>
       </c>
@@ -5653,7 +5656,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A11" s="55" t="s">
         <v>12</v>
       </c>
@@ -5847,7 +5850,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A12" s="55" t="s">
         <v>13</v>
       </c>
@@ -6041,7 +6044,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A13" s="55" t="s">
         <v>232</v>
       </c>
@@ -6235,7 +6238,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A14" s="55" t="s">
         <v>233</v>
       </c>
@@ -6429,7 +6432,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A15" s="55" t="s">
         <v>253</v>
       </c>
@@ -6623,7 +6626,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A16" s="55" t="s">
         <v>254</v>
       </c>
@@ -6817,7 +6820,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="78" t="s">
         <v>307</v>
       </c>
@@ -7011,7 +7014,7 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="55" t="s">
         <v>308</v>
       </c>
@@ -7205,17 +7208,17 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A21" s="57" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.35">
       <c r="B22" s="102" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A23" s="55" t="s">
         <v>47</v>
       </c>
@@ -7224,10 +7227,10 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="D23" s="103" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A24" s="55" t="s">
         <v>157</v>
       </c>
@@ -7236,10 +7239,10 @@
         <v>0.28571428571428575</v>
       </c>
       <c r="D24" s="103" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A25" s="55" t="s">
         <v>322</v>
       </c>
@@ -7248,7 +7251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:64" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="84" t="s">
         <v>262</v>
       </c>
@@ -7358,7 +7361,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="28" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="55" t="s">
         <v>309</v>
       </c>
@@ -7488,7 +7491,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="71" t="s">
         <v>310</v>
       </c>
@@ -7598,7 +7601,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="72" t="s">
         <v>305</v>
       </c>
@@ -7708,7 +7711,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="55" t="s">
         <v>229</v>
       </c>
@@ -7818,7 +7821,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A32" s="55" t="s">
         <v>230</v>
       </c>
@@ -7928,7 +7931,7 @@
         <v>7.5533333333333323E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A33" s="55" t="s">
         <v>306</v>
       </c>
@@ -8038,7 +8041,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A34" s="55" t="s">
         <v>10</v>
       </c>
@@ -8148,7 +8151,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A35" s="55" t="s">
         <v>11</v>
       </c>
@@ -8258,7 +8261,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A36" s="55" t="s">
         <v>12</v>
       </c>
@@ -8368,7 +8371,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A37" s="55" t="s">
         <v>13</v>
       </c>
@@ -8478,7 +8481,7 @@
         <v>8.0052500000000002E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A38" s="55" t="s">
         <v>232</v>
       </c>
@@ -8588,7 +8591,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A39" s="55" t="s">
         <v>233</v>
       </c>
@@ -8698,7 +8701,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A40" s="55" t="s">
         <v>253</v>
       </c>
@@ -8808,7 +8811,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A41" s="55" t="s">
         <v>254</v>
       </c>
@@ -8918,7 +8921,7 @@
         <v>1.8433249999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="78" t="s">
         <v>307</v>
       </c>
@@ -9028,7 +9031,7 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="55" t="s">
         <v>308</v>
       </c>
@@ -9138,15 +9141,18 @@
         <v>2.1746999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A45" s="55" t="s">
+        <v>348</v>
+      </c>
+      <c r="L45" s="55" t="s">
         <v>336</v>
       </c>
       <c r="V45" s="55" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="46" spans="1:39" ht="75" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A46" s="84" t="s">
         <v>262</v>
       </c>
@@ -9163,7 +9169,7 @@
         <v>329</v>
       </c>
       <c r="F46" s="85" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G46" s="85" t="s">
         <v>318</v>
@@ -9174,6 +9180,33 @@
       <c r="I46" s="85" t="s">
         <v>328</v>
       </c>
+      <c r="L46" s="84" t="s">
+        <v>262</v>
+      </c>
+      <c r="M46" s="85" t="s">
+        <v>314</v>
+      </c>
+      <c r="N46" s="85" t="s">
+        <v>319</v>
+      </c>
+      <c r="O46" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="P46" s="85" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q46" s="85" t="s">
+        <v>337</v>
+      </c>
+      <c r="R46" s="85" t="s">
+        <v>318</v>
+      </c>
+      <c r="S46" s="85" t="s">
+        <v>324</v>
+      </c>
+      <c r="T46" s="85" t="s">
+        <v>328</v>
+      </c>
       <c r="V46" s="84" t="s">
         <v>262</v>
       </c>
@@ -9190,7 +9223,7 @@
         <v>329</v>
       </c>
       <c r="AA46" s="85" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB46" s="85" t="s">
         <v>318</v>
@@ -9202,7 +9235,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A47" s="55" t="s">
         <v>309</v>
       </c>
@@ -9237,43 +9270,78 @@
         <f t="array" ref="I47:I62">(Q28:Q43+2*P28:P43)/2</f>
         <v>7.1309142857142863E-2</v>
       </c>
+      <c r="L47" s="55" t="s">
+        <v>309</v>
+      </c>
+      <c r="M47" s="56">
+        <f t="array" ref="M47:M62">((X28:X43+Y28:Y43) +X28:X43)/2</f>
+        <v>0.14676349999999999</v>
+      </c>
+      <c r="N47" s="56">
+        <f t="array" ref="N47:N62">(AC28:AC43*2+AD28:AD43)/2</f>
+        <v>3.0508500000000001E-2</v>
+      </c>
+      <c r="O47" s="56">
+        <f t="array" ref="O47:O62">AH28:AH43</f>
+        <v>7.8895000000000007E-2</v>
+      </c>
+      <c r="P47" s="56">
+        <f t="array" ref="P47:P62">AM28:AM43</f>
+        <v>7.5533333333333323E-4</v>
+      </c>
+      <c r="Q47" s="56">
+        <f t="array" ref="Q47:Q62">W28:W43</f>
+        <v>0.78637999999999997</v>
+      </c>
+      <c r="R47" s="56">
+        <f t="array" ref="R47:R62">(AA28:AA43+AB28:AB43)/2</f>
+        <v>0.1615095</v>
+      </c>
+      <c r="S47" s="56">
+        <f t="array" ref="S47:S62">(AG28:AG43+2*AE28:AE43)/2</f>
+        <v>0.46084099999999995</v>
+      </c>
+      <c r="T47" s="56">
+        <f t="array" ref="T47:T62">(AL28:AL43+2*AK28:AK43)/2</f>
+        <v>0.12066450000000001</v>
+      </c>
       <c r="V47" s="55" t="s">
         <v>309</v>
       </c>
       <c r="W47" s="56">
-        <f t="array" ref="W47:W62">((X28:X43+Y28:Y43) +X28:X43)/2</f>
-        <v>0.14676349999999999</v>
+        <f t="array" ref="W47:W62">0.8*M47:M62</f>
+        <v>0.1174108</v>
       </c>
       <c r="X47" s="56">
-        <f t="array" ref="X47:X62">(AC28:AC43*2+AD28:AD43)/2</f>
-        <v>3.0508500000000001E-2</v>
+        <f t="array" ref="X47:X62">0.8*N47:N62</f>
+        <v>2.4406800000000003E-2</v>
       </c>
       <c r="Y47" s="56">
-        <f t="array" ref="Y47:Y62">AH28:AH43</f>
-        <v>7.8895000000000007E-2</v>
+        <f t="array" ref="Y47:Y62">0.8*O47:O62</f>
+        <v>6.3116000000000005E-2</v>
       </c>
       <c r="Z47" s="56">
-        <f t="array" ref="Z47:Z62">AM28:AM43</f>
-        <v>7.5533333333333323E-4</v>
+        <f t="array" ref="Z47:Z62">0.8*P47:P62</f>
+        <v>6.0426666666666665E-4</v>
       </c>
       <c r="AA47" s="56">
-        <f t="array" ref="AA47:AA62">W28:W43</f>
-        <v>0.78637999999999997</v>
+        <f t="array" ref="AA47:AA62">0.8*Q47:Q62</f>
+        <v>0.629104</v>
       </c>
       <c r="AB47" s="56">
-        <f t="array" ref="AB47:AB62">(AA28:AA43+AB28:AB43)/2</f>
-        <v>0.1615095</v>
+        <f t="array" ref="AB47:AB62">0.8*R47:R62</f>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC47" s="56">
-        <f t="array" ref="AC47:AC62">(AG28:AG43+2*AE28:AE43)/2</f>
-        <v>0.46084099999999995</v>
+        <f t="array" ref="AC47:AC62">0.8*S47:S62</f>
+        <v>0.36867279999999997</v>
       </c>
       <c r="AD47" s="56">
-        <f t="array" ref="AD47:AD62">(AL28:AL43+2*AK28:AK43)/2</f>
-        <v>0.12066450000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+        <f t="array" ref="AD47:AD62">0.8*T47:T62</f>
+        <v>9.6531600000000009E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A48" s="71" t="s">
         <v>310</v>
       </c>
@@ -9301,35 +9369,62 @@
       <c r="I48" s="56">
         <v>7.1309142857142863E-2</v>
       </c>
+      <c r="L48" s="71" t="s">
+        <v>310</v>
+      </c>
+      <c r="M48" s="56">
+        <v>0.14676349999999999</v>
+      </c>
+      <c r="N48" s="56">
+        <v>3.0508500000000001E-2</v>
+      </c>
+      <c r="O48" s="56">
+        <v>7.8895000000000007E-2</v>
+      </c>
+      <c r="P48" s="56">
+        <v>7.5533333333333323E-4</v>
+      </c>
+      <c r="Q48" s="56">
+        <v>0.78637999999999997</v>
+      </c>
+      <c r="R48" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S48" s="56">
+        <v>0.46084099999999995</v>
+      </c>
+      <c r="T48" s="56">
+        <v>0.12066450000000001</v>
+      </c>
       <c r="V48" s="71" t="s">
         <v>310</v>
       </c>
       <c r="W48" s="56">
-        <v>0.14676349999999999</v>
+        <v>0.1174108</v>
       </c>
       <c r="X48" s="56">
-        <v>3.0508500000000001E-2</v>
+        <v>2.4406800000000003E-2</v>
       </c>
       <c r="Y48" s="56">
-        <v>7.8895000000000007E-2</v>
+        <v>6.3116000000000005E-2</v>
       </c>
       <c r="Z48" s="56">
-        <v>7.5533333333333323E-4</v>
+        <v>6.0426666666666665E-4</v>
       </c>
       <c r="AA48" s="56">
-        <v>0.78637999999999997</v>
+        <v>0.629104</v>
       </c>
       <c r="AB48" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC48" s="56">
-        <v>0.46084099999999995</v>
+        <v>0.36867279999999997</v>
       </c>
       <c r="AD48" s="56">
-        <v>0.12066450000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+        <v>9.6531600000000009E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" s="72" t="s">
         <v>305</v>
       </c>
@@ -9357,35 +9452,62 @@
       <c r="I49" s="56">
         <v>7.1309142857142863E-2</v>
       </c>
+      <c r="L49" s="72" t="s">
+        <v>305</v>
+      </c>
+      <c r="M49" s="56">
+        <v>0.14676349999999999</v>
+      </c>
+      <c r="N49" s="56">
+        <v>3.0508500000000001E-2</v>
+      </c>
+      <c r="O49" s="56">
+        <v>7.8895000000000007E-2</v>
+      </c>
+      <c r="P49" s="56">
+        <v>7.5533333333333323E-4</v>
+      </c>
+      <c r="Q49" s="56">
+        <v>0.78637999999999997</v>
+      </c>
+      <c r="R49" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S49" s="56">
+        <v>0.46084099999999995</v>
+      </c>
+      <c r="T49" s="56">
+        <v>0.12066450000000001</v>
+      </c>
       <c r="V49" s="72" t="s">
         <v>305</v>
       </c>
       <c r="W49" s="56">
-        <v>0.14676349999999999</v>
+        <v>0.1174108</v>
       </c>
       <c r="X49" s="56">
-        <v>3.0508500000000001E-2</v>
+        <v>2.4406800000000003E-2</v>
       </c>
       <c r="Y49" s="56">
-        <v>7.8895000000000007E-2</v>
+        <v>6.3116000000000005E-2</v>
       </c>
       <c r="Z49" s="56">
-        <v>7.5533333333333323E-4</v>
+        <v>6.0426666666666665E-4</v>
       </c>
       <c r="AA49" s="56">
-        <v>0.78637999999999997</v>
+        <v>0.629104</v>
       </c>
       <c r="AB49" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC49" s="56">
-        <v>0.46084099999999995</v>
+        <v>0.36867279999999997</v>
       </c>
       <c r="AD49" s="56">
-        <v>0.12066450000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+        <v>9.6531600000000009E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A50" s="55" t="s">
         <v>229</v>
       </c>
@@ -9413,35 +9535,62 @@
       <c r="I50" s="56">
         <v>7.1309142857142863E-2</v>
       </c>
+      <c r="L50" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="M50" s="56">
+        <v>0.14676349999999999</v>
+      </c>
+      <c r="N50" s="56">
+        <v>3.0508500000000001E-2</v>
+      </c>
+      <c r="O50" s="56">
+        <v>7.8895000000000007E-2</v>
+      </c>
+      <c r="P50" s="56">
+        <v>7.5533333333333323E-4</v>
+      </c>
+      <c r="Q50" s="56">
+        <v>0.78637999999999997</v>
+      </c>
+      <c r="R50" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S50" s="56">
+        <v>0.46084099999999995</v>
+      </c>
+      <c r="T50" s="56">
+        <v>0.12066450000000001</v>
+      </c>
       <c r="V50" s="55" t="s">
         <v>229</v>
       </c>
       <c r="W50" s="56">
-        <v>0.14676349999999999</v>
+        <v>0.1174108</v>
       </c>
       <c r="X50" s="56">
-        <v>3.0508500000000001E-2</v>
+        <v>2.4406800000000003E-2</v>
       </c>
       <c r="Y50" s="56">
-        <v>7.8895000000000007E-2</v>
+        <v>6.3116000000000005E-2</v>
       </c>
       <c r="Z50" s="56">
-        <v>7.5533333333333323E-4</v>
+        <v>6.0426666666666665E-4</v>
       </c>
       <c r="AA50" s="56">
-        <v>0.78637999999999997</v>
+        <v>0.629104</v>
       </c>
       <c r="AB50" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC50" s="56">
-        <v>0.46084099999999995</v>
+        <v>0.36867279999999997</v>
       </c>
       <c r="AD50" s="56">
-        <v>0.12066450000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+        <v>9.6531600000000009E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" s="55" t="s">
         <v>230</v>
       </c>
@@ -9469,35 +9618,62 @@
       <c r="I51" s="56">
         <v>7.1309142857142863E-2</v>
       </c>
+      <c r="L51" s="55" t="s">
+        <v>230</v>
+      </c>
+      <c r="M51" s="56">
+        <v>0.14676349999999999</v>
+      </c>
+      <c r="N51" s="56">
+        <v>3.0508500000000001E-2</v>
+      </c>
+      <c r="O51" s="56">
+        <v>7.8895000000000007E-2</v>
+      </c>
+      <c r="P51" s="56">
+        <v>7.5533333333333323E-4</v>
+      </c>
+      <c r="Q51" s="56">
+        <v>0.78637999999999997</v>
+      </c>
+      <c r="R51" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S51" s="56">
+        <v>0.46084099999999995</v>
+      </c>
+      <c r="T51" s="56">
+        <v>0.12066450000000001</v>
+      </c>
       <c r="V51" s="55" t="s">
         <v>230</v>
       </c>
       <c r="W51" s="56">
-        <v>0.14676349999999999</v>
+        <v>0.1174108</v>
       </c>
       <c r="X51" s="56">
-        <v>3.0508500000000001E-2</v>
+        <v>2.4406800000000003E-2</v>
       </c>
       <c r="Y51" s="56">
-        <v>7.8895000000000007E-2</v>
+        <v>6.3116000000000005E-2</v>
       </c>
       <c r="Z51" s="56">
-        <v>7.5533333333333323E-4</v>
+        <v>6.0426666666666665E-4</v>
       </c>
       <c r="AA51" s="56">
-        <v>0.78637999999999997</v>
+        <v>0.629104</v>
       </c>
       <c r="AB51" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC51" s="56">
-        <v>0.46084099999999995</v>
+        <v>0.36867279999999997</v>
       </c>
       <c r="AD51" s="56">
-        <v>0.12066450000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+        <v>9.6531600000000009E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" s="55" t="s">
         <v>306</v>
       </c>
@@ -9525,35 +9701,62 @@
       <c r="I52" s="56">
         <v>5.3409928571428567E-2</v>
       </c>
+      <c r="L52" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="M52" s="56">
+        <v>7.678299999999999E-2</v>
+      </c>
+      <c r="N52" s="56">
+        <v>3.5521374999999994E-2</v>
+      </c>
+      <c r="O52" s="56">
+        <v>0.1312325</v>
+      </c>
+      <c r="P52" s="56">
+        <v>8.0052500000000002E-3</v>
+      </c>
+      <c r="Q52" s="56">
+        <v>0.62775775</v>
+      </c>
+      <c r="R52" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S52" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T52" s="56">
+        <v>9.0632875000000002E-2</v>
+      </c>
       <c r="V52" s="55" t="s">
         <v>306</v>
       </c>
       <c r="W52" s="56">
-        <v>7.678299999999999E-2</v>
+        <v>6.1426399999999992E-2</v>
       </c>
       <c r="X52" s="56">
-        <v>3.5521374999999994E-2</v>
+        <v>2.8417099999999997E-2</v>
       </c>
       <c r="Y52" s="56">
-        <v>0.1312325</v>
+        <v>0.10498600000000001</v>
       </c>
       <c r="Z52" s="56">
-        <v>8.0052500000000002E-3</v>
+        <v>6.4042000000000005E-3</v>
       </c>
       <c r="AA52" s="56">
-        <v>0.62775775</v>
+        <v>0.50220620000000005</v>
       </c>
       <c r="AB52" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC52" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD52" s="56">
-        <v>9.0632875000000002E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+        <v>7.250630000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" s="55" t="s">
         <v>10</v>
       </c>
@@ -9581,35 +9784,62 @@
       <c r="I53" s="56">
         <v>5.3409928571428567E-2</v>
       </c>
+      <c r="L53" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="M53" s="56">
+        <v>7.678299999999999E-2</v>
+      </c>
+      <c r="N53" s="56">
+        <v>3.5521374999999994E-2</v>
+      </c>
+      <c r="O53" s="56">
+        <v>0.1312325</v>
+      </c>
+      <c r="P53" s="56">
+        <v>8.0052500000000002E-3</v>
+      </c>
+      <c r="Q53" s="56">
+        <v>0.62775775</v>
+      </c>
+      <c r="R53" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S53" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T53" s="56">
+        <v>9.0632875000000002E-2</v>
+      </c>
       <c r="V53" s="55" t="s">
         <v>10</v>
       </c>
       <c r="W53" s="56">
-        <v>7.678299999999999E-2</v>
+        <v>6.1426399999999992E-2</v>
       </c>
       <c r="X53" s="56">
-        <v>3.5521374999999994E-2</v>
+        <v>2.8417099999999997E-2</v>
       </c>
       <c r="Y53" s="56">
-        <v>0.1312325</v>
+        <v>0.10498600000000001</v>
       </c>
       <c r="Z53" s="56">
-        <v>8.0052500000000002E-3</v>
+        <v>6.4042000000000005E-3</v>
       </c>
       <c r="AA53" s="56">
-        <v>0.62775775</v>
+        <v>0.50220620000000005</v>
       </c>
       <c r="AB53" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC53" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD53" s="56">
-        <v>9.0632875000000002E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+        <v>7.250630000000001E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" s="55" t="s">
         <v>11</v>
       </c>
@@ -9637,35 +9867,62 @@
       <c r="I54" s="56">
         <v>5.3409928571428567E-2</v>
       </c>
+      <c r="L54" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="M54" s="56">
+        <v>7.678299999999999E-2</v>
+      </c>
+      <c r="N54" s="56">
+        <v>3.5521374999999994E-2</v>
+      </c>
+      <c r="O54" s="56">
+        <v>0.1312325</v>
+      </c>
+      <c r="P54" s="56">
+        <v>8.0052500000000002E-3</v>
+      </c>
+      <c r="Q54" s="56">
+        <v>0.62775775</v>
+      </c>
+      <c r="R54" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S54" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T54" s="56">
+        <v>9.0632875000000002E-2</v>
+      </c>
       <c r="V54" s="55" t="s">
         <v>11</v>
       </c>
       <c r="W54" s="56">
-        <v>7.678299999999999E-2</v>
+        <v>6.1426399999999992E-2</v>
       </c>
       <c r="X54" s="56">
-        <v>3.5521374999999994E-2</v>
+        <v>2.8417099999999997E-2</v>
       </c>
       <c r="Y54" s="56">
-        <v>0.1312325</v>
+        <v>0.10498600000000001</v>
       </c>
       <c r="Z54" s="56">
-        <v>8.0052500000000002E-3</v>
+        <v>6.4042000000000005E-3</v>
       </c>
       <c r="AA54" s="56">
-        <v>0.62775775</v>
+        <v>0.50220620000000005</v>
       </c>
       <c r="AB54" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC54" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD54" s="56">
-        <v>9.0632875000000002E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+        <v>7.250630000000001E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" s="55" t="s">
         <v>12</v>
       </c>
@@ -9693,35 +9950,62 @@
       <c r="I55" s="56">
         <v>5.3409928571428567E-2</v>
       </c>
+      <c r="L55" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="M55" s="56">
+        <v>7.678299999999999E-2</v>
+      </c>
+      <c r="N55" s="56">
+        <v>3.5521374999999994E-2</v>
+      </c>
+      <c r="O55" s="56">
+        <v>0.1312325</v>
+      </c>
+      <c r="P55" s="56">
+        <v>8.0052500000000002E-3</v>
+      </c>
+      <c r="Q55" s="56">
+        <v>0.62775775</v>
+      </c>
+      <c r="R55" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S55" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T55" s="56">
+        <v>9.0632875000000002E-2</v>
+      </c>
       <c r="V55" s="55" t="s">
         <v>12</v>
       </c>
       <c r="W55" s="56">
-        <v>7.678299999999999E-2</v>
+        <v>6.1426399999999992E-2</v>
       </c>
       <c r="X55" s="56">
-        <v>3.5521374999999994E-2</v>
+        <v>2.8417099999999997E-2</v>
       </c>
       <c r="Y55" s="56">
-        <v>0.1312325</v>
+        <v>0.10498600000000001</v>
       </c>
       <c r="Z55" s="56">
-        <v>8.0052500000000002E-3</v>
+        <v>6.4042000000000005E-3</v>
       </c>
       <c r="AA55" s="56">
-        <v>0.62775775</v>
+        <v>0.50220620000000005</v>
       </c>
       <c r="AB55" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC55" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD55" s="56">
-        <v>9.0632875000000002E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+        <v>7.250630000000001E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" s="55" t="s">
         <v>13</v>
       </c>
@@ -9749,35 +10033,62 @@
       <c r="I56" s="56">
         <v>5.3409928571428567E-2</v>
       </c>
+      <c r="L56" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="M56" s="56">
+        <v>7.678299999999999E-2</v>
+      </c>
+      <c r="N56" s="56">
+        <v>3.5521374999999994E-2</v>
+      </c>
+      <c r="O56" s="56">
+        <v>0.1312325</v>
+      </c>
+      <c r="P56" s="56">
+        <v>8.0052500000000002E-3</v>
+      </c>
+      <c r="Q56" s="56">
+        <v>0.62775775</v>
+      </c>
+      <c r="R56" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S56" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T56" s="56">
+        <v>9.0632875000000002E-2</v>
+      </c>
       <c r="V56" s="55" t="s">
         <v>13</v>
       </c>
       <c r="W56" s="56">
-        <v>7.678299999999999E-2</v>
+        <v>6.1426399999999992E-2</v>
       </c>
       <c r="X56" s="56">
-        <v>3.5521374999999994E-2</v>
+        <v>2.8417099999999997E-2</v>
       </c>
       <c r="Y56" s="56">
-        <v>0.1312325</v>
+        <v>0.10498600000000001</v>
       </c>
       <c r="Z56" s="56">
-        <v>8.0052500000000002E-3</v>
+        <v>6.4042000000000005E-3</v>
       </c>
       <c r="AA56" s="56">
-        <v>0.62775775</v>
+        <v>0.50220620000000005</v>
       </c>
       <c r="AB56" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC56" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD56" s="56">
-        <v>9.0632875000000002E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+        <v>7.250630000000001E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" s="55" t="s">
         <v>232</v>
       </c>
@@ -9805,35 +10116,62 @@
       <c r="I57" s="56">
         <v>1.9593678571428571E-2</v>
       </c>
+      <c r="L57" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="M57" s="56">
+        <v>5.6984E-2</v>
+      </c>
+      <c r="N57" s="56">
+        <v>4.4296500000000003E-2</v>
+      </c>
+      <c r="O57" s="56">
+        <v>0.17620050000000001</v>
+      </c>
+      <c r="P57" s="56">
+        <v>1.8433249999999998E-2</v>
+      </c>
+      <c r="Q57" s="56">
+        <v>0.40971574999999999</v>
+      </c>
+      <c r="R57" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S57" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T57" s="56">
+        <v>3.3547999999999994E-2</v>
+      </c>
       <c r="V57" s="55" t="s">
         <v>232</v>
       </c>
       <c r="W57" s="56">
-        <v>5.6984E-2</v>
+        <v>4.5587200000000001E-2</v>
       </c>
       <c r="X57" s="56">
-        <v>4.4296500000000003E-2</v>
+        <v>3.5437200000000002E-2</v>
       </c>
       <c r="Y57" s="56">
-        <v>0.17620050000000001</v>
+        <v>0.14096040000000001</v>
       </c>
       <c r="Z57" s="56">
-        <v>1.8433249999999998E-2</v>
+        <v>1.4746599999999999E-2</v>
       </c>
       <c r="AA57" s="56">
-        <v>0.40971574999999999</v>
+        <v>0.32777260000000003</v>
       </c>
       <c r="AB57" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC57" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD57" s="56">
-        <v>3.3547999999999994E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+        <v>2.6838399999999998E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" s="55" t="s">
         <v>233</v>
       </c>
@@ -9861,35 +10199,62 @@
       <c r="I58" s="56">
         <v>1.9593678571428571E-2</v>
       </c>
+      <c r="L58" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="M58" s="56">
+        <v>5.6984E-2</v>
+      </c>
+      <c r="N58" s="56">
+        <v>4.4296500000000003E-2</v>
+      </c>
+      <c r="O58" s="56">
+        <v>0.17620050000000001</v>
+      </c>
+      <c r="P58" s="56">
+        <v>1.8433249999999998E-2</v>
+      </c>
+      <c r="Q58" s="56">
+        <v>0.40971574999999999</v>
+      </c>
+      <c r="R58" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S58" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T58" s="56">
+        <v>3.3547999999999994E-2</v>
+      </c>
       <c r="V58" s="55" t="s">
         <v>233</v>
       </c>
       <c r="W58" s="56">
-        <v>5.6984E-2</v>
+        <v>4.5587200000000001E-2</v>
       </c>
       <c r="X58" s="56">
-        <v>4.4296500000000003E-2</v>
+        <v>3.5437200000000002E-2</v>
       </c>
       <c r="Y58" s="56">
-        <v>0.17620050000000001</v>
+        <v>0.14096040000000001</v>
       </c>
       <c r="Z58" s="56">
-        <v>1.8433249999999998E-2</v>
+        <v>1.4746599999999999E-2</v>
       </c>
       <c r="AA58" s="56">
-        <v>0.40971574999999999</v>
+        <v>0.32777260000000003</v>
       </c>
       <c r="AB58" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC58" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD58" s="56">
-        <v>3.3547999999999994E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+        <v>2.6838399999999998E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" s="55" t="s">
         <v>253</v>
       </c>
@@ -9917,35 +10282,62 @@
       <c r="I59" s="56">
         <v>1.9593678571428571E-2</v>
       </c>
+      <c r="L59" s="55" t="s">
+        <v>253</v>
+      </c>
+      <c r="M59" s="56">
+        <v>5.6984E-2</v>
+      </c>
+      <c r="N59" s="56">
+        <v>4.4296500000000003E-2</v>
+      </c>
+      <c r="O59" s="56">
+        <v>0.17620050000000001</v>
+      </c>
+      <c r="P59" s="56">
+        <v>1.8433249999999998E-2</v>
+      </c>
+      <c r="Q59" s="56">
+        <v>0.40971574999999999</v>
+      </c>
+      <c r="R59" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S59" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T59" s="56">
+        <v>3.3547999999999994E-2</v>
+      </c>
       <c r="V59" s="55" t="s">
         <v>253</v>
       </c>
       <c r="W59" s="56">
-        <v>5.6984E-2</v>
+        <v>4.5587200000000001E-2</v>
       </c>
       <c r="X59" s="56">
-        <v>4.4296500000000003E-2</v>
+        <v>3.5437200000000002E-2</v>
       </c>
       <c r="Y59" s="56">
-        <v>0.17620050000000001</v>
+        <v>0.14096040000000001</v>
       </c>
       <c r="Z59" s="56">
-        <v>1.8433249999999998E-2</v>
+        <v>1.4746599999999999E-2</v>
       </c>
       <c r="AA59" s="56">
-        <v>0.40971574999999999</v>
+        <v>0.32777260000000003</v>
       </c>
       <c r="AB59" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC59" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD59" s="56">
-        <v>3.3547999999999994E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+        <v>2.6838399999999998E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" s="55" t="s">
         <v>254</v>
       </c>
@@ -9973,35 +10365,62 @@
       <c r="I60" s="56">
         <v>1.9593678571428571E-2</v>
       </c>
+      <c r="L60" s="55" t="s">
+        <v>254</v>
+      </c>
+      <c r="M60" s="56">
+        <v>5.6984E-2</v>
+      </c>
+      <c r="N60" s="56">
+        <v>4.4296500000000003E-2</v>
+      </c>
+      <c r="O60" s="56">
+        <v>0.17620050000000001</v>
+      </c>
+      <c r="P60" s="56">
+        <v>1.8433249999999998E-2</v>
+      </c>
+      <c r="Q60" s="56">
+        <v>0.40971574999999999</v>
+      </c>
+      <c r="R60" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S60" s="56">
+        <v>0.460841</v>
+      </c>
+      <c r="T60" s="56">
+        <v>3.3547999999999994E-2</v>
+      </c>
       <c r="V60" s="55" t="s">
         <v>254</v>
       </c>
       <c r="W60" s="56">
-        <v>5.6984E-2</v>
+        <v>4.5587200000000001E-2</v>
       </c>
       <c r="X60" s="56">
-        <v>4.4296500000000003E-2</v>
+        <v>3.5437200000000002E-2</v>
       </c>
       <c r="Y60" s="56">
-        <v>0.17620050000000001</v>
+        <v>0.14096040000000001</v>
       </c>
       <c r="Z60" s="56">
-        <v>1.8433249999999998E-2</v>
+        <v>1.4746599999999999E-2</v>
       </c>
       <c r="AA60" s="56">
-        <v>0.40971574999999999</v>
+        <v>0.32777260000000003</v>
       </c>
       <c r="AB60" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC60" s="56">
-        <v>0.460841</v>
+        <v>0.36867280000000002</v>
       </c>
       <c r="AD60" s="56">
-        <v>3.3547999999999994E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+        <v>2.6838399999999998E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" s="78" t="s">
         <v>307</v>
       </c>
@@ -10029,35 +10448,62 @@
       <c r="I61" s="56">
         <v>9.9361666666666678E-3</v>
       </c>
+      <c r="L61" s="78" t="s">
+        <v>307</v>
+      </c>
+      <c r="M61" s="56">
+        <v>5.6984E-2</v>
+      </c>
+      <c r="N61" s="56">
+        <v>4.4296500000000003E-2</v>
+      </c>
+      <c r="O61" s="56">
+        <v>0.20378033333333334</v>
+      </c>
+      <c r="P61" s="56">
+        <v>2.1746999999999999E-2</v>
+      </c>
+      <c r="Q61" s="56">
+        <v>0.36699399999999999</v>
+      </c>
+      <c r="R61" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S61" s="56">
+        <v>0.46084099999999995</v>
+      </c>
+      <c r="T61" s="56">
+        <v>1.7070999999999999E-2</v>
+      </c>
       <c r="V61" s="78" t="s">
         <v>307</v>
       </c>
       <c r="W61" s="56">
-        <v>5.6984E-2</v>
+        <v>4.5587200000000001E-2</v>
       </c>
       <c r="X61" s="56">
-        <v>4.4296500000000003E-2</v>
+        <v>3.5437200000000002E-2</v>
       </c>
       <c r="Y61" s="56">
-        <v>0.20378033333333334</v>
+        <v>0.1630242666666667</v>
       </c>
       <c r="Z61" s="56">
-        <v>2.1746999999999999E-2</v>
+        <v>1.7397599999999999E-2</v>
       </c>
       <c r="AA61" s="56">
-        <v>0.36699399999999999</v>
+        <v>0.2935952</v>
       </c>
       <c r="AB61" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC61" s="56">
-        <v>0.46084099999999995</v>
+        <v>0.36867279999999997</v>
       </c>
       <c r="AD61" s="56">
-        <v>1.7070999999999999E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+        <v>1.36568E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" s="55" t="s">
         <v>308</v>
       </c>
@@ -10085,36 +10531,63 @@
       <c r="I62" s="56">
         <v>9.9361666666666678E-3</v>
       </c>
+      <c r="L62" s="55" t="s">
+        <v>308</v>
+      </c>
+      <c r="M62" s="56">
+        <v>5.6984E-2</v>
+      </c>
+      <c r="N62" s="56">
+        <v>4.4296500000000003E-2</v>
+      </c>
+      <c r="O62" s="56">
+        <v>0.20378033333333334</v>
+      </c>
+      <c r="P62" s="56">
+        <v>2.1746999999999999E-2</v>
+      </c>
+      <c r="Q62" s="56">
+        <v>0.36699399999999999</v>
+      </c>
+      <c r="R62" s="56">
+        <v>0.1615095</v>
+      </c>
+      <c r="S62" s="56">
+        <v>0.46084099999999995</v>
+      </c>
+      <c r="T62" s="56">
+        <v>1.7070999999999999E-2</v>
+      </c>
       <c r="V62" s="55" t="s">
         <v>308</v>
       </c>
       <c r="W62" s="56">
-        <v>5.6984E-2</v>
+        <v>4.5587200000000001E-2</v>
       </c>
       <c r="X62" s="56">
-        <v>4.4296500000000003E-2</v>
+        <v>3.5437200000000002E-2</v>
       </c>
       <c r="Y62" s="56">
-        <v>0.20378033333333334</v>
+        <v>0.1630242666666667</v>
       </c>
       <c r="Z62" s="56">
-        <v>2.1746999999999999E-2</v>
+        <v>1.7397599999999999E-2</v>
       </c>
       <c r="AA62" s="56">
-        <v>0.36699399999999999</v>
+        <v>0.2935952</v>
       </c>
       <c r="AB62" s="56">
-        <v>0.1615095</v>
+        <v>0.12920760000000001</v>
       </c>
       <c r="AC62" s="56">
-        <v>0.46084099999999995</v>
+        <v>0.36867279999999997</v>
       </c>
       <c r="AD62" s="56">
-        <v>1.7070999999999999E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.36568E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="86"/>
       <c r="B67" s="87"/>
       <c r="C67" s="88" t="s">
@@ -10122,7 +10595,7 @@
       </c>
       <c r="D67" s="89"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="90"/>
       <c r="C68" s="91" t="s">
         <v>201</v>
@@ -10132,7 +10605,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="90"/>
       <c r="C69" s="91" t="s">
         <v>241</v>
@@ -10142,7 +10615,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="90"/>
       <c r="C70" s="91" t="s">
         <v>199</v>
@@ -10152,7 +10625,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="94"/>
       <c r="B71" s="95"/>
       <c r="C71" s="96" t="s">
@@ -10163,12 +10636,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="55" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="98" t="s">
         <v>201</v>
       </c>
@@ -10179,7 +10652,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="90" t="s">
         <v>241</v>
       </c>
@@ -10190,7 +10663,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="90" t="s">
         <v>199</v>
       </c>
@@ -10198,7 +10671,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="94" t="s">
         <v>198</v>
       </c>
@@ -10206,12 +10679,12 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="55" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="98" t="s">
         <v>201</v>
       </c>
@@ -10222,7 +10695,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="90" t="s">
         <v>241</v>
       </c>
@@ -10233,7 +10706,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="90" t="s">
         <v>199</v>
       </c>
@@ -10244,7 +10717,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="94" t="s">
         <v>198</v>
       </c>
@@ -10255,7 +10728,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D85" s="57" t="s">
         <v>250</v>
       </c>
@@ -10278,27 +10751,27 @@
       <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" customWidth="1"/>
-    <col min="20" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.1796875" customWidth="1"/>
+    <col min="20" max="23" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.54296875" customWidth="1"/>
     <col min="26" max="26" width="32" customWidth="1"/>
-    <col min="27" max="29" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.42578125" customWidth="1"/>
+    <col min="27" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="12" t="s">
         <v>58</v>
       </c>
@@ -10325,7 +10798,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>57</v>
       </c>
@@ -10380,7 +10853,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>60</v>
       </c>
@@ -10442,7 +10915,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
@@ -10498,7 +10971,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>106</v>
       </c>
@@ -10533,7 +11006,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B6" s="15"/>
       <c r="M6" s="4" t="s">
         <v>114</v>
@@ -10572,7 +11045,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="M7" s="3" t="s">
         <v>118</v>
       </c>
@@ -10603,7 +11076,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="S8" s="3" t="s">
         <v>129</v>
       </c>
@@ -10628,7 +11101,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="Y9" s="3" t="s">
         <v>138</v>
       </c>
@@ -10636,12 +11109,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="AD10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="S11" s="24" t="s">
         <v>130</v>
       </c>
@@ -10652,7 +11125,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="K12" s="15"/>
       <c r="T12" s="24" t="s">
         <v>124</v>
@@ -10669,7 +11142,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="S13" s="21" t="s">
         <v>119</v>
       </c>
@@ -10692,7 +11165,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="S14" s="13" t="s">
         <v>120</v>
       </c>
@@ -10709,7 +11182,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="S15" s="13" t="s">
         <v>121</v>
       </c>
@@ -10722,7 +11195,7 @@
       </c>
       <c r="W15" s="4"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="S16" s="13" t="s">
         <v>122</v>
       </c>
@@ -10741,7 +11214,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="17" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S17" s="13" t="s">
         <v>123</v>
       </c>
@@ -10761,18 +11234,18 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S18" s="3" t="s">
         <v>129</v>
       </c>
       <c r="AA18" s="15"/>
     </row>
-    <row r="20" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S20" s="24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="19:27" x14ac:dyDescent="0.35">
       <c r="T21" s="24" t="s">
         <v>124</v>
       </c>
@@ -10782,7 +11255,7 @@
       </c>
       <c r="W21" s="24"/>
     </row>
-    <row r="22" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S22" s="21" t="s">
         <v>119</v>
       </c>
@@ -10799,7 +11272,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S23" s="13" t="s">
         <v>120</v>
       </c>
@@ -10816,7 +11289,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="24" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S24" s="13" t="s">
         <v>121</v>
       </c>
@@ -10829,7 +11302,7 @@
       </c>
       <c r="W24" s="4"/>
     </row>
-    <row r="25" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S25" s="13" t="s">
         <v>123</v>
       </c>
@@ -10846,7 +11319,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="26" spans="19:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="19:27" x14ac:dyDescent="0.35">
       <c r="S26" s="3" t="s">
         <v>129</v>
       </c>
@@ -10867,16 +11340,16 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -10893,7 +11366,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -10940,7 +11413,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -10988,7 +11461,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -11030,7 +11503,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -11063,7 +11536,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -11093,7 +11566,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -11114,7 +11587,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -11141,7 +11614,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -11169,7 +11642,7 @@
         <v>0.13824884792626729</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
@@ -11194,7 +11667,7 @@
         <v>9.8360655737704916E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -11212,10 +11685,10 @@
         <v>7.6E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>261</v>
       </c>
@@ -11232,23 +11705,23 @@
         <v>1.8800000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>332</v>
       </c>
@@ -11259,9 +11732,9 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B24" s="41">
         <v>8.0070000000000002E-3</v>
@@ -11273,9 +11746,9 @@
         <v>6.6827999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B25" s="41">
         <v>9.7230000000000007E-3</v>
@@ -11287,9 +11760,9 @@
         <v>8.1147999999999998E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B26" s="41">
         <v>1.1802999999999999E-2</v>
@@ -11304,9 +11777,9 @@
         <v>258</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B27" s="41">
         <v>1.4298999999999999E-2</v>
@@ -11318,9 +11791,9 @@
         <v>0.119336</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B28" s="41">
         <v>8.0070000000000002E-3</v>
@@ -11332,7 +11805,7 @@
         <v>6.6827999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -11346,10 +11819,10 @@
         <v>4.3395000000000003E-2</v>
       </c>
       <c r="E29" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E30" t="s">
         <v>335</v>
       </c>
@@ -11369,28 +11842,28 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.5703125" customWidth="1"/>
-    <col min="25" max="25" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.5703125" customWidth="1"/>
-    <col min="31" max="31" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.54296875" customWidth="1"/>
+    <col min="25" max="25" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.54296875" customWidth="1"/>
+    <col min="31" max="31" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -11415,7 +11888,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -11478,7 +11951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -11542,7 +12015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
@@ -11606,7 +12079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -11646,7 +12119,7 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>38</v>
       </c>
@@ -11699,7 +12172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -11741,7 +12214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -11780,7 +12253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -11804,7 +12277,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -11837,7 +12310,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -11879,7 +12352,7 @@
         <v>0.74550000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -11908,7 +12381,7 @@
         <v>0.751</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -11939,7 +12412,7 @@
         <v>0.24271844660194175</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -11963,7 +12436,7 @@
         <v>0.12376237623762376</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="H15" s="7"/>
       <c r="N15" s="4" t="s">
         <v>67</v>
@@ -11981,21 +12454,21 @@
         <v>7.1225071225071226E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="H16" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
@@ -12003,7 +12476,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
@@ -12014,7 +12487,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
@@ -12025,12 +12498,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>47</v>
       </c>
@@ -12041,7 +12514,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>1</v>
       </c>
@@ -12058,7 +12531,7 @@
         <v>9.0833333333333339E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
@@ -12075,22 +12548,22 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
         <v>141</v>
       </c>
@@ -12098,7 +12571,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B37" s="22" t="s">
         <v>62</v>
       </c>
@@ -12118,7 +12591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>83</v>
       </c>
@@ -12147,7 +12620,7 @@
         <v>7.5000000000000002E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>88</v>
       </c>
@@ -12176,7 +12649,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
         <v>89</v>
       </c>
@@ -12205,7 +12678,7 @@
         <v>1.7499999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>91</v>
       </c>
@@ -12235,7 +12708,7 @@
         <v>3.2500000000000003E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
         <v>142</v>
       </c>
@@ -12243,7 +12716,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B44" s="22" t="s">
         <v>62</v>
       </c>
@@ -12263,7 +12736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>83</v>
       </c>
@@ -12292,7 +12765,7 @@
         <v>1.25E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>88</v>
       </c>
@@ -12321,7 +12794,7 @@
         <v>3.4999999999999996E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
         <v>89</v>
       </c>
@@ -12350,7 +12823,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
         <v>91</v>
       </c>
@@ -12379,21 +12852,21 @@
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>90</v>
       </c>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G51" s="23"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
         <v>92</v>
       </c>
@@ -12407,7 +12880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
         <v>96</v>
       </c>
@@ -12421,7 +12894,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
         <v>94</v>
       </c>
@@ -12435,7 +12908,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
         <v>95</v>
       </c>
@@ -12449,12 +12922,12 @@
         <v>13.42</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
         <v>92</v>
       </c>
@@ -12468,7 +12941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
         <v>96</v>
       </c>
@@ -12482,7 +12955,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
         <v>94</v>
       </c>
@@ -12496,7 +12969,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
         <v>95</v>
       </c>
@@ -12526,14 +12999,14 @@
       <selection activeCell="B3" sqref="B3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>237</v>
       </c>
@@ -12541,7 +13014,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
         <v>229</v>
       </c>
@@ -12555,7 +13028,7 @@
         <v>16.6279069767441</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -12569,7 +13042,7 @@
         <v>39.999999999999901</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>231</v>
       </c>
@@ -12583,7 +13056,7 @@
         <v>45.232558139534802</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -12597,7 +13070,7 @@
         <v>43.139534883720899</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -12611,7 +13084,7 @@
         <v>39.651162790697597</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -12625,7 +13098,7 @@
         <v>24.651162790697601</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Ading age standardized outputs
</commit_message>
<xml_diff>
--- a/HPVData.xlsx
+++ b/HPVData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="HPV" sheetId="6" r:id="rId1"/>
@@ -2790,8 +2790,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3896,8 +3896,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BL85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O43" workbookViewId="0">
-      <selection activeCell="AF58" sqref="AF58"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Removing files and scripts that are no longer used
</commit_message>
<xml_diff>
--- a/HPVData.xlsx
+++ b/HPVData.xlsx
@@ -1157,7 +1157,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1173,6 +1173,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1829,7 +1835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1960,6 +1966,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2790,8 +2797,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3604,11 +3611,11 @@
       <c r="G29" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="26">
+      <c r="H29" s="104">
         <f>1/24.3*12</f>
         <v>0.49382716049382713</v>
       </c>
-      <c r="I29" s="26">
+      <c r="I29" s="104">
         <v>0.75774999999999992</v>
       </c>
       <c r="Q29" t="s">
@@ -3628,11 +3635,11 @@
       <c r="G30" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="104">
         <f>1/24.3*12</f>
         <v>0.49382716049382713</v>
       </c>
-      <c r="I30" s="26">
+      <c r="I30" s="104">
         <v>1</v>
       </c>
       <c r="Q30" t="s">
@@ -3652,11 +3659,11 @@
       <c r="G31" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="H31" s="26">
+      <c r="H31" s="104">
         <f>MIN(H29:H30)</f>
         <v>0.49382716049382713</v>
       </c>
-      <c r="I31" s="26">
+      <c r="I31" s="104">
         <f>MIN(I29:I30)</f>
         <v>0.75774999999999992</v>
       </c>

</xml_diff>